<commit_message>
Version with corrected substrate values, number of steady state simulation changed to 500 and disturbance feeding on scenario 1b corrected so OLR is no more than 1.2
</commit_message>
<xml_diff>
--- a/documentation/variation_coefficients.xlsx
+++ b/documentation/variation_coefficients.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shellmann\SimonsHardDriveSpeicher\GIT\ad_meal_prep_control\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanma\Documents\GitHub\ad_meal_prep_control\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908AAB7B-554E-467C-BB2D-1A5B377E1DF0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA2058A-8A15-426F-9015-EC84E6275C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{FEC59851-A8F1-448C-AC8E-0F026119D9F7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FEC59851-A8F1-448C-AC8E-0F026119D9F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -70,12 +70,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -90,11 +96,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -110,9 +117,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -150,7 +157,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -256,7 +263,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -398,7 +405,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -409,12 +416,12 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -425,56 +432,56 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>1.94</v>
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>5.52</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>8.23</v>
+        <v>6</v>
+      </c>
+      <c r="B3" s="1">
+        <v>10.039999999999999</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>7.4</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>5.52</v>
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>8.23</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>10.039999999999999</v>
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.94</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -482,5 +489,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update variation coefficients for BMP
</commit_message>
<xml_diff>
--- a/documentation/variation_coefficients.xlsx
+++ b/documentation/variation_coefficients.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanma\Documents\GitHub\ad_meal_prep_control\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shellmann\SimonsHardDriveSpeicher\GIT\ad_meal_prep_control\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA2058A-8A15-426F-9015-EC84E6275C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFB1233-C953-4114-9AF7-BC0B64835F73}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FEC59851-A8F1-448C-AC8E-0F026119D9F7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" xr2:uid="{FEC59851-A8F1-448C-AC8E-0F026119D9F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
     <t>Delory (2025) (submitted)</t>
   </si>
   <si>
-    <t>Hafner (2018) (mean of all 4 substrates, using robust mean and SD)</t>
+    <t>Hafner (2020), Tab. 3 (mean of all 4 substrates SA-SD without cellulose)</t>
   </si>
 </sst>
 </file>
@@ -101,7 +101,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -117,9 +117,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -157,7 +157,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -263,7 +263,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -405,7 +405,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -416,12 +416,12 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -432,7 +432,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -443,7 +443,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -454,7 +454,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -465,18 +465,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>8.23</v>
+        <v>14.51</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>

</xml_diff>